<commit_message>
class Signal rewrited with @property and @.setter
</commit_message>
<xml_diff>
--- a/input.xlsx
+++ b/input.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="1853" yWindow="0" windowWidth="22264" windowHeight="12647"/>
+    <workbookView xWindow="2780" yWindow="0" windowWidth="22264" windowHeight="12647"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -84,12 +84,6 @@
     <t>Weintek_Position</t>
   </si>
   <si>
-    <t>IZV_addr</t>
-  </si>
-  <si>
-    <t>OPV_addr</t>
-  </si>
-  <si>
     <t>TUSH_addr</t>
   </si>
   <si>
@@ -120,7 +114,13 @@
     <t>MOV_addr</t>
   </si>
   <si>
-    <t>XSY_addr</t>
+    <t>DI_M_addr</t>
+  </si>
+  <si>
+    <t>DO_M_addr</t>
+  </si>
+  <si>
+    <t>DO_NM_addr</t>
   </si>
 </sst>
 </file>
@@ -567,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="AA5" sqref="AA5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -595,9 +595,9 @@
     <col min="20" max="20" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="9" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="8" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.5546875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="10.77734375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9.44140625" bestFit="1" customWidth="1"/>
@@ -653,7 +653,7 @@
         <v>13</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="P1" s="7" t="s">
         <v>14</v>
@@ -677,40 +677,40 @@
         <v>20</v>
       </c>
       <c r="W1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="8" t="s">
+      <c r="AB1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="AC1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="Y1" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z1" s="8" t="s">
+      <c r="AD1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="AA1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="AC1" s="8" t="s">
+      <c r="AE1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="8" t="s">
+      <c r="AF1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="8" t="s">
+      <c r="AG1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:34" ht="15.65" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>